<commit_message>
updated with Q4 2024 results
</commit_message>
<xml_diff>
--- a/data/Auto_Metrics.xlsx
+++ b/data/Auto_Metrics.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:D199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2939,6 +2939,1406 @@
         </is>
       </c>
     </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B130">
+        <v>94.2</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B131">
+        <v>68.90000000000001</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B132">
+        <v>74.3</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B133">
+        <v>-0.5</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B134">
+        <v>25.3</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B135">
+        <v>-4.9</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B136">
+        <v>1575</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B137">
+        <v>97</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B138">
+        <v>14.2</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B139">
+        <v>96.09999999999999</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B140">
+        <v>95.40000000000001</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B141">
+        <v>69.59999999999999</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B142">
+        <v>71.8</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B143">
+        <v>1.6</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B144">
+        <v>25.8</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B145">
+        <v>-3.8</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B146">
+        <v>6640</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B147">
+        <v>5956</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B148">
+        <v>306</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B149">
+        <v>292</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B150">
+        <v>94.7</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B151">
+        <v>68.90000000000001</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B152">
+        <v>74.3</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B153">
+        <v>1.1</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B154">
+        <v>25.8</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B155">
+        <v>-6.5</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B156">
+        <v>95.2</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B157">
+        <v>69.8</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B158">
+        <v>75.8</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B159">
+        <v>-0.1</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B160">
+        <v>25.4</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B161">
+        <v>-5.9</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B162">
+        <v>1408</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B163">
+        <v>74</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B164">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B165">
+        <v>95.90000000000001</v>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B166">
+        <v>71.2</v>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B167">
+        <v>70.40000000000001</v>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B168">
+        <v>71.3</v>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B169">
+        <v>71.5</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B170">
+        <v>1.1</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B171">
+        <v>0.1</v>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B172">
+        <v>25.7</v>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B173">
+        <v>24.7</v>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B174">
+        <v>-1.4</v>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B175">
+        <v>-1</v>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B176">
+        <v>438.7</v>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B177">
+        <v>416</v>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B178">
+        <v>16.2</v>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B179">
+        <v>16.8</v>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B180">
+        <v>10.6</v>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Q4 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B181">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Q4 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B182">
+        <v>98.3</v>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B183">
+        <v>96.7</v>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B184">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B185">
+        <v>71.8</v>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B186">
+        <v>72.59999999999999</v>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B187">
+        <v>70.90000000000001</v>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B188">
+        <v>1.1</v>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B189">
+        <v>0.9</v>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B190">
+        <v>26.5</v>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B191">
+        <v>25.6</v>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B192">
+        <v>-0.9</v>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B193">
+        <v>-1.7</v>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B194">
+        <v>1657.1</v>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B195">
+        <v>1867.4</v>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B196">
+        <v>54.9</v>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B197">
+        <v>26.5</v>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B198">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B199">
+        <v>10.6</v>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>